<commit_message>
update results for paper
</commit_message>
<xml_diff>
--- a/Experiment results process/CNNTProjectionEvaluation.xlsx
+++ b/Experiment results process/CNNTProjectionEvaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\li.7957\Desktop\Map_Identification_Classification\Experiment results process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiali\Desktop\Map_Identification_Classification\Experiment results process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73E3998-E405-40FD-8277-B3630CB0CBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD216E56-6238-4B7B-BA0C-6A8BB605969C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B8C258A4-480A-4177-AC24-72CBE0817F24}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{B8C258A4-480A-4177-AC24-72CBE0817F24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,12 +400,15 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="7" max="7" width="13.765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,7 +422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -445,7 +448,7 @@
         <v>0.85213414634146334</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -471,7 +474,7 @@
         <v>0.93509350935093516</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -497,7 +500,7 @@
         <v>0.93310463121783882</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -523,7 +526,7 @@
         <v>0.98969072164948457</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -549,7 +552,7 @@
         <v>0.98901098901098905</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F7">
         <f>SUM(F2:F6)/5</f>
         <v>0.94013801537386443</v>

</xml_diff>